<commit_message>
Incorporate battery storage files from RMI
</commit_message>
<xml_diff>
--- a/InputData/elec/BGrBSC/BAU Grid Battery Storage Cap.xlsx
+++ b/InputData/elec/BGrBSC/BAU Grid Battery Storage Cap.xlsx
@@ -8507,7 +8507,7 @@
         <v>2021</v>
       </c>
       <c r="B9" s="28" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -8515,7 +8515,7 @@
         <v>2022</v>
       </c>
       <c r="B10" s="28" t="n">
-        <v>0</v>
+        <v>17.79361362691557</v>
       </c>
     </row>
     <row r="11">
@@ -8523,7 +8523,7 @@
         <v>2023</v>
       </c>
       <c r="B11" s="28" t="n">
-        <v>0</v>
+        <v>19.58723009632501</v>
       </c>
     </row>
     <row r="12">
@@ -8531,7 +8531,7 @@
         <v>2024</v>
       </c>
       <c r="B12" s="28" t="n">
-        <v>0</v>
+        <v>21.37800122937859</v>
       </c>
     </row>
     <row r="13">
@@ -8539,7 +8539,7 @@
         <v>2025</v>
       </c>
       <c r="B13" s="28" t="n">
-        <v>0</v>
+        <v>22.63722601024008</v>
       </c>
     </row>
     <row r="14">
@@ -8547,7 +8547,7 @@
         <v>2026</v>
       </c>
       <c r="B14" s="28" t="n">
-        <v>0</v>
+        <v>23.8054909875179</v>
       </c>
     </row>
     <row r="15">
@@ -8555,7 +8555,7 @@
         <v>2027</v>
       </c>
       <c r="B15" s="28" t="n">
-        <v>0</v>
+        <v>24.97375596479571</v>
       </c>
     </row>
     <row r="16">
@@ -8563,7 +8563,7 @@
         <v>2028</v>
       </c>
       <c r="B16" s="28" t="n">
-        <v>0</v>
+        <v>26.14202094207353</v>
       </c>
     </row>
     <row r="17">
@@ -8571,7 +8571,7 @@
         <v>2029</v>
       </c>
       <c r="B17" s="28" t="n">
-        <v>0</v>
+        <v>27.45519909892944</v>
       </c>
     </row>
     <row r="18">
@@ -8579,7 +8579,7 @@
         <v>2030</v>
       </c>
       <c r="B18" s="28" t="n">
-        <v>0</v>
+        <v>28.62346407620726</v>
       </c>
     </row>
     <row r="19">
@@ -8587,7 +8587,7 @@
         <v>2031</v>
       </c>
       <c r="B19" s="28" t="n">
-        <v>0</v>
+        <v>28.62346407620726</v>
       </c>
     </row>
     <row r="20">
@@ -8595,7 +8595,7 @@
         <v>2032</v>
       </c>
       <c r="B20" s="28" t="n">
-        <v>0</v>
+        <v>28.62346407620726</v>
       </c>
     </row>
     <row r="21">
@@ -8603,7 +8603,7 @@
         <v>2033</v>
       </c>
       <c r="B21" s="28" t="n">
-        <v>0</v>
+        <v>29.43932803445102</v>
       </c>
     </row>
     <row r="22">
@@ -8611,7 +8611,7 @@
         <v>2034</v>
       </c>
       <c r="B22" s="28" t="n">
-        <v>0</v>
+        <v>30.71186137157435</v>
       </c>
     </row>
     <row r="23">
@@ -8619,7 +8619,7 @@
         <v>2035</v>
       </c>
       <c r="B23" s="28" t="n">
-        <v>0</v>
+        <v>30.71186137157435</v>
       </c>
     </row>
     <row r="24">
@@ -8627,7 +8627,7 @@
         <v>2036</v>
       </c>
       <c r="B24" s="28" t="n">
-        <v>0</v>
+        <v>30.90396847674307</v>
       </c>
     </row>
     <row r="25">
@@ -8635,7 +8635,7 @@
         <v>2037</v>
       </c>
       <c r="B25" s="28" t="n">
-        <v>0</v>
+        <v>30.90396847674307</v>
       </c>
     </row>
     <row r="26">
@@ -8643,7 +8643,7 @@
         <v>2038</v>
       </c>
       <c r="B26" s="28" t="n">
-        <v>0</v>
+        <v>30.94603738590052</v>
       </c>
     </row>
     <row r="27">
@@ -8651,7 +8651,7 @@
         <v>2039</v>
       </c>
       <c r="B27" s="28" t="n">
-        <v>0</v>
+        <v>30.94603738590052</v>
       </c>
     </row>
     <row r="28">
@@ -8659,7 +8659,7 @@
         <v>2040</v>
       </c>
       <c r="B28" s="28" t="n">
-        <v>0</v>
+        <v>31.19432638225146</v>
       </c>
     </row>
     <row r="29">
@@ -8667,7 +8667,7 @@
         <v>2041</v>
       </c>
       <c r="B29" s="28" t="n">
-        <v>0</v>
+        <v>32.44331534271593</v>
       </c>
     </row>
     <row r="30">
@@ -8675,7 +8675,7 @@
         <v>2042</v>
       </c>
       <c r="B30" s="28" t="n">
-        <v>0</v>
+        <v>34.13381466229396</v>
       </c>
     </row>
     <row r="31">
@@ -8683,7 +8683,7 @@
         <v>2043</v>
       </c>
       <c r="B31" s="28" t="n">
-        <v>0</v>
+        <v>34.13381466229396</v>
       </c>
     </row>
     <row r="32">
@@ -8691,7 +8691,7 @@
         <v>2044</v>
       </c>
       <c r="B32" s="28" t="n">
-        <v>0</v>
+        <v>34.13381466229396</v>
       </c>
     </row>
     <row r="33">
@@ -8699,7 +8699,7 @@
         <v>2045</v>
       </c>
       <c r="B33" s="28" t="n">
-        <v>0</v>
+        <v>35.93554929417324</v>
       </c>
     </row>
     <row r="34">
@@ -8707,7 +8707,7 @@
         <v>2046</v>
       </c>
       <c r="B34" s="28" t="n">
-        <v>0</v>
+        <v>37.86672825403367</v>
       </c>
     </row>
     <row r="35">
@@ -8715,7 +8715,7 @@
         <v>2047</v>
       </c>
       <c r="B35" s="28" t="n">
-        <v>0</v>
+        <v>42.86956293103754</v>
       </c>
     </row>
     <row r="36">
@@ -8723,7 +8723,7 @@
         <v>2048</v>
       </c>
       <c r="B36" s="28" t="n">
-        <v>0</v>
+        <v>45.71492486933411</v>
       </c>
     </row>
     <row r="37">
@@ -8731,7 +8731,7 @@
         <v>2049</v>
       </c>
       <c r="B37" s="28" t="n">
-        <v>0</v>
+        <v>49.36304971166452</v>
       </c>
     </row>
     <row r="38">
@@ -8739,7 +8739,7 @@
         <v>2050</v>
       </c>
       <c r="B38" s="28" t="n">
-        <v>0</v>
+        <v>49.46194007312315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>